<commit_message>
Added better support for sparsely populated objects
</commit_message>
<xml_diff>
--- a/examples/basic-sheet-output.xlsx
+++ b/examples/basic-sheet-output.xlsx
@@ -397,8 +397,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="b">
-        <v>0</v>
+      <c r="A3" t="str">
+        <v/>
       </c>
       <c r="B3" t="str">
         <v>Paul</v>

</xml_diff>